<commit_message>
added Categories Table to RecordCount.sql
</commit_message>
<xml_diff>
--- a/AlgoDB/AlgoDB_Management.xlsx
+++ b/AlgoDB/AlgoDB_Management.xlsx
@@ -76,7 +76,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId13"/>
+    <pivotCache cacheId="2" r:id="rId13"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -339,7 +339,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="483">
   <si>
     <t>GBPUSD</t>
   </si>
@@ -1751,9 +1751,6 @@
     <t>FOREX</t>
   </si>
   <si>
-    <t>STOCKS</t>
-  </si>
-  <si>
     <t>BONDS</t>
   </si>
   <si>
@@ -1788,6 +1785,9 @@
   </si>
   <si>
     <t>union</t>
+  </si>
+  <si>
+    <t>INDICES</t>
   </si>
 </sst>
 </file>
@@ -2066,301 +2066,301 @@
   </cellStyles>
   <dxfs count="284">
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="yyyy/mm/dd\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="yyyy/mm/dd\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2369,7 +2369,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -2381,10 +2381,10 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2393,7 +2393,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <fill>
@@ -2404,7 +2404,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2413,133 +2413,133 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2548,7 +2548,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -2560,10 +2560,10 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2572,7 +2572,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <fill>
@@ -2583,7 +2583,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2592,133 +2592,133 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2727,7 +2727,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -2739,10 +2739,10 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2751,7 +2751,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <fill>
@@ -2762,7 +2762,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2771,133 +2771,133 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2906,7 +2906,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -2918,10 +2918,10 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2930,7 +2930,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <fill>
@@ -2941,7 +2941,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2950,88 +2950,88 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3047,7 +3047,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="gcaglion" refreshedDate="43490.441992476852" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="168">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="felicini" refreshedDate="43687.706460532405" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="56">
   <cacheSource type="external" connectionId="41"/>
   <cacheFields count="9">
     <cacheField name="TABLENAME" numFmtId="0" sqlType="12">
@@ -3055,31 +3055,31 @@
     </cacheField>
     <cacheField name="SYMBOL" numFmtId="0" sqlType="12">
       <sharedItems count="25">
-        <s v="AUDUSD"/>
-        <s v="CATTLE"/>
-        <s v="CORN"/>
         <s v="ETXEUR"/>
         <s v="EURUSD"/>
-        <s v="FTSE"/>
-        <s v="GBPNZD"/>
         <s v="GBPUSD"/>
-        <s v="HOIL"/>
-        <s v="NGAS"/>
-        <s v="NZDUSD"/>
-        <s v="OIL"/>
-        <s v="PLATINUM"/>
-        <s v="RICE"/>
-        <s v="SBO"/>
-        <s v="SOYBEANS"/>
         <s v="SPX"/>
-        <s v="SUGAR"/>
         <s v="US10YR"/>
         <s v="USDJPY"/>
-        <s v="WHEAT"/>
         <s v="WTIUSD"/>
         <s v="XAUUSD"/>
-        <s v="XRB"/>
+        <s v="CORN" u="1"/>
+        <s v="HOIL" u="1"/>
+        <s v="SUGAR" u="1"/>
+        <s v="AUDUSD" u="1"/>
+        <s v="SOYBEANS" u="1"/>
+        <s v="CATTLE" u="1"/>
+        <s v="NZDUSD" u="1"/>
+        <s v="OIL" u="1"/>
         <s v="GOLD" u="1"/>
+        <s v="NGAS" u="1"/>
+        <s v="PLATINUM" u="1"/>
+        <s v="SBO" u="1"/>
+        <s v="XRB" u="1"/>
+        <s v="RICE" u="1"/>
+        <s v="WHEAT" u="1"/>
+        <s v="FTSE" u="1"/>
+        <s v="GBPNZD" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="TIMEFRAME" numFmtId="0" sqlType="12">
@@ -3101,106 +3101,97 @@
       </sharedItems>
     </cacheField>
     <cacheField name="TOTALCOUNT" numFmtId="0" sqlType="6">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="6160868"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="6166608" count="27">
+        <n v="2072"/>
+        <n v="29065"/>
+        <n v="0"/>
+        <n v="1277846"/>
+        <n v="5701"/>
+        <n v="113029"/>
+        <n v="6166608"/>
+        <n v="5704"/>
+        <n v="113036"/>
+        <n v="6051930"/>
+        <n v="2518"/>
+        <n v="48996"/>
+        <n v="2117667"/>
+        <n v="7856"/>
+        <n v="25305"/>
+        <n v="544614"/>
+        <n v="74100"/>
+        <n v="43183"/>
+        <n v="5706"/>
+        <n v="113123"/>
+        <n v="6129662"/>
+        <n v="2520"/>
+        <n v="48486"/>
+        <n v="2555385"/>
+        <n v="3050"/>
+        <n v="59342"/>
+        <n v="3447353"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="MINDATE" numFmtId="0" sqlType="11">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2000-05-30T00:00:00" maxDate="2010-11-16T00:00:00" count="29">
-        <d v="2000-06-05T00:00:00"/>
-        <d v="2000-06-05T12:00:00"/>
-        <d v="2000-06-05T12:03:00"/>
-        <m/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="1982-05-03T23:59:00" maxDate="2010-11-16T00:00:00" count="19">
         <d v="2010-11-15T00:00:00"/>
         <d v="2010-11-15T02:00:00"/>
+        <m/>
         <d v="2000-05-30T00:00:00"/>
         <d v="2000-05-30T17:00:00"/>
-        <d v="2000-05-30T16:00:00"/>
         <d v="2000-05-30T17:27:00"/>
-        <d v="2000-05-30T17:15:00"/>
-        <d v="2000-05-30T17:25:00"/>
-        <d v="2008-03-30T00:00:00"/>
-        <d v="2008-03-30T17:00:00"/>
-        <d v="2008-03-30T16:00:00"/>
         <d v="2000-05-30T17:59:00"/>
-        <d v="2005-08-12T00:00:00"/>
-        <d v="2005-08-12T17:00:00"/>
-        <d v="2005-08-12T16:00:00"/>
-        <d v="2005-08-12T17:01:00"/>
         <d v="2010-11-14T00:00:00"/>
         <d v="2010-11-14T18:00:00"/>
-        <d v="2010-11-14T16:00:00"/>
+        <d v="1982-05-03T23:59:00"/>
+        <d v="1998-04-13T16:00:00"/>
+        <d v="1998-04-13T15:03:00"/>
+        <d v="1998-04-13T15:15:00"/>
+        <d v="1998-04-13T15:30:00"/>
         <d v="2000-05-30T17:58:00"/>
         <d v="2010-11-14T20:00:00"/>
         <d v="2010-11-14T20:15:00"/>
         <d v="2009-03-15T00:00:00"/>
         <d v="2009-03-15T17:00:00"/>
-        <d v="2009-03-15T16:00:00"/>
       </sharedItems>
     </cacheField>
     <cacheField name="MAXDATE" numFmtId="0" sqlType="11">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2015-12-24T12:00:00" maxDate="2018-12-31T16:59:00" count="27">
-        <d v="2017-12-28T00:00:00"/>
-        <d v="2015-12-24T12:00:00"/>
-        <d v="2017-12-29T12:00:00"/>
-        <d v="2018-12-31T16:58:00"/>
-        <m/>
-        <d v="2017-10-27T16:50:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2013-07-12T15:02:00" maxDate="2018-12-31T16:59:00" count="15">
         <d v="2018-12-28T00:00:00"/>
         <d v="2018-12-31T06:00:00"/>
-        <d v="2018-12-31T00:00:00"/>
+        <m/>
         <d v="2018-12-31T07:58:00"/>
-        <d v="2018-12-31T07:30:00"/>
-        <d v="2018-12-31T07:00:00"/>
-        <d v="2018-12-31T07:50:00"/>
         <d v="2018-12-30T00:00:00"/>
         <d v="2018-12-31T15:00:00"/>
-        <d v="2018-12-31T12:00:00"/>
         <d v="2018-12-31T16:59:00"/>
-        <d v="2018-12-31T16:30:00"/>
-        <d v="2018-12-31T16:00:00"/>
-        <d v="2018-12-31T16:50:00"/>
-        <d v="2017-12-29T15:00:00"/>
+        <d v="2018-12-31T16:58:00"/>
         <d v="2018-12-31T16:13:00"/>
-        <d v="2018-12-31T15:45:00"/>
-        <d v="2018-12-31T15:30:00"/>
-        <d v="2018-12-31T16:05:00"/>
+        <d v="2013-07-12T23:59:00"/>
+        <d v="2013-07-12T16:00:00"/>
+        <d v="2013-07-12T15:02:00"/>
+        <d v="2013-07-12T15:15:00"/>
+        <d v="2013-07-12T15:30:00"/>
         <d v="2018-12-31T16:16:00"/>
-        <d v="2018-12-31T16:10:00"/>
       </sharedItems>
     </cacheField>
     <cacheField name="SYMBOL2" numFmtId="0" sqlType="12">
-      <sharedItems count="24">
-        <s v="AUDUSD"/>
-        <s v="CATTLE"/>
-        <s v="CORN"/>
+      <sharedItems count="8">
         <s v="ETXEUR"/>
         <s v="EURUSD"/>
-        <s v="FTSE"/>
-        <s v="GBPNZD"/>
         <s v="GBPUSD"/>
-        <s v="HOIL"/>
-        <s v="NGAS"/>
-        <s v="NZDUSD"/>
-        <s v="OIL"/>
-        <s v="PLATINUM"/>
-        <s v="RICE"/>
-        <s v="SBO"/>
-        <s v="SOYBEANS"/>
         <s v="SPX"/>
-        <s v="SUGAR"/>
         <s v="US10YR"/>
         <s v="USDJPY"/>
-        <s v="WHEAT"/>
         <s v="WTIUSD"/>
         <s v="XAUUSD"/>
-        <s v="XRB"/>
       </sharedItems>
     </cacheField>
     <cacheField name="CATEGORY" numFmtId="0" sqlType="12">
-      <sharedItems count="4">
+      <sharedItems count="5">
+        <s v="INDICES"/>
         <s v="FOREX"/>
+        <s v="BONDS"/>
         <s v="COMMODITIES"/>
-        <s v="STOCKS"/>
-        <s v="BONDS"/>
+        <s v="STOCKS" u="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -3213,1890 +3204,658 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="168">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="56">
   <r>
-    <s v="AUDUSD_D1"/>
+    <s v="ETXEUR_D1"/>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="5139"/>
+    <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
   </r>
   <r>
-    <s v="AUDUSD_H1"/>
+    <s v="ETXEUR_H1"/>
     <x v="0"/>
     <x v="1"/>
     <x v="0"/>
-    <n v="88174"/>
+    <x v="1"/>
     <x v="1"/>
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
   </r>
   <r>
-    <s v="AUDUSD_H4"/>
+    <s v="ETXEUR_H4"/>
     <x v="0"/>
     <x v="2"/>
     <x v="0"/>
-    <n v="26145"/>
-    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
   </r>
   <r>
-    <s v="AUDUSD_M1"/>
+    <s v="ETXEUR_M1"/>
     <x v="0"/>
     <x v="3"/>
     <x v="0"/>
-    <n v="5525543"/>
-    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
     <x v="3"/>
     <x v="0"/>
     <x v="0"/>
   </r>
   <r>
-    <s v="AUDUSD_M15"/>
+    <s v="ETXEUR_M15"/>
     <x v="0"/>
     <x v="4"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="0"/>
     <x v="0"/>
   </r>
   <r>
-    <s v="AUDUSD_M30"/>
+    <s v="ETXEUR_M30"/>
     <x v="0"/>
     <x v="5"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="0"/>
     <x v="0"/>
   </r>
   <r>
-    <s v="AUDUSD_M5"/>
+    <s v="ETXEUR_M5"/>
     <x v="0"/>
     <x v="6"/>
     <x v="0"/>
-    <n v="1161021"/>
-    <x v="1"/>
-    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="0"/>
     <x v="0"/>
   </r>
   <r>
-    <s v="CATTLE_D1"/>
+    <s v="EURUSD_D1"/>
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="0"/>
+    <x v="4"/>
     <x v="3"/>
     <x v="4"/>
     <x v="1"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CATTLE_H1"/>
+    <s v="EURUSD_H1"/>
     <x v="1"/>
     <x v="1"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
+    <x v="5"/>
     <x v="4"/>
+    <x v="5"/>
     <x v="1"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CATTLE_H4"/>
+    <s v="EURUSD_H4"/>
     <x v="1"/>
     <x v="2"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CATTLE_M1"/>
+    <s v="EURUSD_M1"/>
     <x v="1"/>
     <x v="3"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="6"/>
     <x v="1"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CATTLE_M15"/>
+    <s v="EURUSD_M15"/>
     <x v="1"/>
     <x v="4"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CATTLE_M30"/>
+    <s v="EURUSD_M30"/>
     <x v="1"/>
     <x v="5"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CATTLE_M5"/>
+    <s v="EURUSD_M5"/>
     <x v="1"/>
     <x v="6"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CORN_D1"/>
+    <s v="GBPUSD_D1"/>
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="0"/>
+    <x v="7"/>
     <x v="3"/>
     <x v="4"/>
     <x v="2"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CORN_H1"/>
+    <s v="GBPUSD_H1"/>
     <x v="2"/>
     <x v="1"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
+    <x v="8"/>
     <x v="4"/>
+    <x v="5"/>
     <x v="2"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CORN_H4"/>
+    <s v="GBPUSD_H4"/>
     <x v="2"/>
     <x v="2"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="2"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CORN_M1"/>
+    <s v="GBPUSD_M1"/>
     <x v="2"/>
     <x v="3"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="9"/>
+    <x v="6"/>
+    <x v="7"/>
     <x v="2"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CORN_M15"/>
+    <s v="GBPUSD_M15"/>
     <x v="2"/>
     <x v="4"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="2"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CORN_M30"/>
+    <s v="GBPUSD_M30"/>
     <x v="2"/>
     <x v="5"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="2"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="CORN_M5"/>
+    <s v="GBPUSD_M5"/>
     <x v="2"/>
     <x v="6"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="2"/>
     <x v="1"/>
   </r>
   <r>
-    <s v="ETXEUR_D1"/>
+    <s v="SPX_D1"/>
     <x v="3"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="2072"/>
+    <x v="10"/>
+    <x v="7"/>
     <x v="4"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="SPX_H1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="8"/>
+    <x v="5"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="SPX_H4"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="SPX_M1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="12"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="SPX_M15"/>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="SPX_M30"/>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="SPX_M5"/>
+    <x v="3"/>
     <x v="6"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="US10YR_D1"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="4"/>
     <x v="2"/>
   </r>
   <r>
-    <s v="ETXEUR_H1"/>
-    <x v="3"/>
+    <s v="US10YR_H1"/>
+    <x v="4"/>
     <x v="1"/>
     <x v="0"/>
-    <n v="29065"/>
-    <x v="5"/>
-    <x v="7"/>
-    <x v="3"/>
+    <x v="14"/>
+    <x v="10"/>
+    <x v="10"/>
+    <x v="4"/>
     <x v="2"/>
   </r>
   <r>
-    <s v="ETXEUR_H4"/>
-    <x v="3"/>
+    <s v="US10YR_H4"/>
+    <x v="4"/>
     <x v="2"/>
     <x v="0"/>
-    <n v="8544"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="4"/>
-    <x v="8"/>
-    <x v="3"/>
     <x v="2"/>
   </r>
   <r>
-    <s v="ETXEUR_M1"/>
-    <x v="3"/>
+    <s v="US10YR_M1"/>
+    <x v="4"/>
     <x v="3"/>
     <x v="0"/>
-    <n v="1277846"/>
-    <x v="5"/>
-    <x v="9"/>
-    <x v="3"/>
+    <x v="15"/>
+    <x v="11"/>
+    <x v="11"/>
+    <x v="4"/>
     <x v="2"/>
   </r>
   <r>
-    <s v="ETXEUR_M15"/>
-    <x v="3"/>
+    <s v="US10YR_M15"/>
+    <x v="4"/>
     <x v="4"/>
     <x v="0"/>
-    <n v="115223"/>
-    <x v="5"/>
-    <x v="10"/>
-    <x v="3"/>
+    <x v="16"/>
+    <x v="12"/>
+    <x v="12"/>
+    <x v="4"/>
     <x v="2"/>
   </r>
   <r>
-    <s v="ETXEUR_M30"/>
-    <x v="3"/>
+    <s v="US10YR_M30"/>
+    <x v="4"/>
     <x v="5"/>
     <x v="0"/>
-    <n v="57921"/>
-    <x v="5"/>
-    <x v="11"/>
-    <x v="3"/>
+    <x v="17"/>
+    <x v="13"/>
+    <x v="13"/>
+    <x v="4"/>
     <x v="2"/>
   </r>
   <r>
-    <s v="ETXEUR_M5"/>
-    <x v="3"/>
+    <s v="US10YR_M5"/>
+    <x v="4"/>
     <x v="6"/>
     <x v="0"/>
-    <n v="332825"/>
-    <x v="5"/>
-    <x v="12"/>
-    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
     <x v="2"/>
   </r>
   <r>
-    <s v="EURUSD_D1"/>
-    <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="5696"/>
-    <x v="6"/>
-    <x v="13"/>
-    <x v="4"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="EURUSD_H1"/>
-    <x v="4"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="112933"/>
-    <x v="7"/>
-    <x v="14"/>
-    <x v="4"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="EURUSD_H4"/>
-    <x v="4"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="29284"/>
-    <x v="8"/>
-    <x v="15"/>
-    <x v="4"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="EURUSD_M1"/>
-    <x v="4"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="6160868"/>
-    <x v="9"/>
-    <x v="16"/>
-    <x v="4"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="EURUSD_M15"/>
-    <x v="4"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="449430"/>
-    <x v="10"/>
-    <x v="17"/>
-    <x v="4"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="EURUSD_M30"/>
-    <x v="4"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="225346"/>
-    <x v="7"/>
-    <x v="18"/>
-    <x v="4"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="EURUSD_M5"/>
-    <x v="4"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="1335673"/>
-    <x v="11"/>
-    <x v="19"/>
-    <x v="4"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="FTSE_D1"/>
+    <s v="USDJPY_D1"/>
     <x v="5"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="0"/>
+    <x v="18"/>
     <x v="3"/>
     <x v="4"/>
     <x v="5"/>
-    <x v="2"/>
+    <x v="1"/>
   </r>
   <r>
-    <s v="FTSE_H1"/>
+    <s v="USDJPY_H1"/>
     <x v="5"/>
     <x v="1"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
+    <x v="19"/>
     <x v="4"/>
     <x v="5"/>
-    <x v="2"/>
+    <x v="5"/>
+    <x v="1"/>
   </r>
   <r>
-    <s v="FTSE_H4"/>
+    <s v="USDJPY_H4"/>
     <x v="5"/>
     <x v="2"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="5"/>
-    <x v="2"/>
+    <x v="1"/>
   </r>
   <r>
-    <s v="FTSE_M1"/>
+    <s v="USDJPY_M1"/>
     <x v="5"/>
     <x v="3"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="20"/>
+    <x v="14"/>
+    <x v="7"/>
     <x v="5"/>
-    <x v="2"/>
+    <x v="1"/>
   </r>
   <r>
-    <s v="FTSE_M15"/>
+    <s v="USDJPY_M15"/>
     <x v="5"/>
     <x v="4"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="5"/>
-    <x v="2"/>
+    <x v="1"/>
   </r>
   <r>
-    <s v="FTSE_M30"/>
+    <s v="USDJPY_M30"/>
     <x v="5"/>
     <x v="5"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="5"/>
-    <x v="2"/>
+    <x v="1"/>
   </r>
   <r>
-    <s v="FTSE_M5"/>
+    <s v="USDJPY_M5"/>
     <x v="5"/>
     <x v="6"/>
     <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="5"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="GBPNZD_D1"/>
-    <x v="6"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="3036"/>
-    <x v="12"/>
-    <x v="0"/>
-    <x v="6"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPNZD_H1"/>
-    <x v="6"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="60478"/>
-    <x v="13"/>
-    <x v="20"/>
-    <x v="6"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPNZD_H4"/>
-    <x v="6"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="15634"/>
-    <x v="14"/>
-    <x v="2"/>
-    <x v="6"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPNZD_M1"/>
-    <x v="6"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="3957732"/>
-    <x v="13"/>
-    <x v="3"/>
-    <x v="6"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPNZD_M15"/>
-    <x v="6"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="6"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPNZD_M30"/>
-    <x v="6"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="6"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPNZD_M5"/>
-    <x v="6"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="6"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPUSD_D1"/>
-    <x v="7"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="5386"/>
-    <x v="6"/>
-    <x v="0"/>
-    <x v="7"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPUSD_H1"/>
-    <x v="7"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="106714"/>
-    <x v="7"/>
-    <x v="20"/>
-    <x v="7"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPUSD_H4"/>
-    <x v="7"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="27679"/>
-    <x v="8"/>
-    <x v="2"/>
-    <x v="7"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPUSD_M1"/>
-    <x v="7"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="6046193"/>
-    <x v="15"/>
-    <x v="3"/>
-    <x v="7"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPUSD_M15"/>
-    <x v="7"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="7"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPUSD_M30"/>
-    <x v="7"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="7"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="GBPUSD_M5"/>
-    <x v="7"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="7"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="HOIL_D1"/>
-    <x v="8"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="8"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="HOIL_H1"/>
-    <x v="8"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="8"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="HOIL_H4"/>
-    <x v="8"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="8"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="HOIL_M1"/>
-    <x v="8"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="8"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="HOIL_M15"/>
-    <x v="8"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="8"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="HOIL_M30"/>
-    <x v="8"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="8"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="HOIL_M5"/>
-    <x v="8"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="8"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="NGAS_D1"/>
-    <x v="9"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="9"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="NGAS_H1"/>
-    <x v="9"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="9"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="NGAS_H4"/>
-    <x v="9"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="9"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="NGAS_M1"/>
-    <x v="9"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="9"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="NGAS_M15"/>
-    <x v="9"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="9"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="NGAS_M30"/>
-    <x v="9"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="9"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="NGAS_M5"/>
-    <x v="9"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="9"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="NZDUSD_D1"/>
-    <x v="10"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="3666"/>
-    <x v="16"/>
-    <x v="0"/>
-    <x v="10"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="NZDUSD_H1"/>
-    <x v="10"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="73075"/>
-    <x v="17"/>
-    <x v="20"/>
-    <x v="10"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="NZDUSD_H4"/>
-    <x v="10"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="18892"/>
-    <x v="18"/>
-    <x v="2"/>
-    <x v="10"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="NZDUSD_M1"/>
-    <x v="10"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="4207343"/>
-    <x v="19"/>
-    <x v="3"/>
-    <x v="10"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="NZDUSD_M15"/>
-    <x v="10"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="10"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="NZDUSD_M30"/>
-    <x v="10"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="10"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="NZDUSD_M5"/>
-    <x v="10"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="10"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="OIL_D1"/>
-    <x v="11"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="11"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="OIL_H1"/>
-    <x v="11"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="11"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="OIL_H4"/>
-    <x v="11"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="11"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="OIL_M1"/>
-    <x v="11"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="11"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="OIL_M15"/>
-    <x v="11"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="11"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="OIL_M30"/>
-    <x v="11"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="11"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="OIL_M5"/>
-    <x v="11"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="11"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="PLATINUM_D1"/>
-    <x v="12"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="12"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="PLATINUM_H1"/>
-    <x v="12"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="12"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="PLATINUM_H4"/>
-    <x v="12"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="12"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="PLATINUM_M1"/>
-    <x v="12"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="12"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="PLATINUM_M15"/>
-    <x v="12"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="12"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="PLATINUM_M30"/>
-    <x v="12"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="12"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="PLATINUM_M5"/>
-    <x v="12"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="12"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="RICE_D1"/>
-    <x v="13"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="13"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="RICE_H1"/>
-    <x v="13"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="13"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="RICE_H4"/>
-    <x v="13"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="13"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="RICE_M1"/>
-    <x v="13"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="13"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="RICE_M15"/>
-    <x v="13"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="13"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="RICE_M30"/>
-    <x v="13"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="13"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="RICE_M5"/>
-    <x v="13"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="13"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SBO_D1"/>
-    <x v="14"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="14"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SBO_H1"/>
-    <x v="14"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="14"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SBO_H4"/>
-    <x v="14"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="14"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SBO_M1"/>
-    <x v="14"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="14"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SBO_M15"/>
-    <x v="14"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="14"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SBO_M30"/>
-    <x v="14"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="14"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SBO_M5"/>
-    <x v="14"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="14"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SOYBEANS_D1"/>
-    <x v="15"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="15"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SOYBEANS_H1"/>
-    <x v="15"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="15"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SOYBEANS_H4"/>
-    <x v="15"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="15"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SOYBEANS_M1"/>
-    <x v="15"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="15"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SOYBEANS_M15"/>
-    <x v="15"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="15"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SOYBEANS_M30"/>
-    <x v="15"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="15"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SOYBEANS_M5"/>
-    <x v="15"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="15"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SPX_D1"/>
-    <x v="16"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="2518"/>
-    <x v="20"/>
-    <x v="13"/>
-    <x v="16"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="SPX_H1"/>
-    <x v="16"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="48996"/>
-    <x v="21"/>
-    <x v="14"/>
-    <x v="16"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="SPX_H4"/>
-    <x v="16"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="12925"/>
-    <x v="22"/>
-    <x v="15"/>
-    <x v="16"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="SPX_M1"/>
-    <x v="16"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="2117667"/>
-    <x v="21"/>
-    <x v="21"/>
-    <x v="16"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="SPX_M15"/>
-    <x v="16"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="190548"/>
-    <x v="21"/>
-    <x v="22"/>
-    <x v="16"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="SPX_M30"/>
-    <x v="16"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="96652"/>
-    <x v="21"/>
-    <x v="23"/>
-    <x v="16"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="SPX_M5"/>
-    <x v="16"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="543097"/>
-    <x v="21"/>
-    <x v="24"/>
-    <x v="16"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <s v="SUGAR_D1"/>
-    <x v="17"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="17"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SUGAR_H1"/>
-    <x v="17"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="17"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SUGAR_H4"/>
-    <x v="17"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="17"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SUGAR_M1"/>
-    <x v="17"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="17"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SUGAR_M15"/>
-    <x v="17"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="17"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SUGAR_M30"/>
-    <x v="17"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="17"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="SUGAR_M5"/>
-    <x v="17"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="17"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="US10YR_D1"/>
-    <x v="18"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="18"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <s v="US10YR_H1"/>
-    <x v="18"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="18"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <s v="US10YR_H4"/>
-    <x v="18"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="18"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <s v="US10YR_M1"/>
-    <x v="18"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="18"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <s v="US10YR_M15"/>
-    <x v="18"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="18"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <s v="US10YR_M30"/>
-    <x v="18"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="18"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <s v="US10YR_M5"/>
-    <x v="18"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="18"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <s v="USDJPY_D1"/>
-    <x v="19"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="5388"/>
-    <x v="6"/>
-    <x v="0"/>
-    <x v="19"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="USDJPY_H1"/>
-    <x v="19"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="106801"/>
-    <x v="7"/>
-    <x v="20"/>
-    <x v="19"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="USDJPY_H4"/>
-    <x v="19"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="27697"/>
-    <x v="8"/>
-    <x v="2"/>
-    <x v="19"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="USDJPY_M1"/>
-    <x v="19"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="6123961"/>
-    <x v="23"/>
-    <x v="3"/>
-    <x v="19"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="USDJPY_M15"/>
-    <x v="19"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="19"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="USDJPY_M30"/>
-    <x v="19"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="19"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="USDJPY_M5"/>
-    <x v="19"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="19"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <s v="WHEAT_D1"/>
-    <x v="20"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="20"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="WHEAT_H1"/>
-    <x v="20"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="20"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="WHEAT_H4"/>
-    <x v="20"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="20"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="WHEAT_M1"/>
-    <x v="20"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="20"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="WHEAT_M15"/>
-    <x v="20"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="20"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="WHEAT_M30"/>
-    <x v="20"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="20"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="WHEAT_M5"/>
-    <x v="20"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="20"/>
     <x v="1"/>
   </r>
   <r>
     <s v="WTIUSD_D1"/>
-    <x v="21"/>
+    <x v="6"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="2520"/>
-    <x v="20"/>
-    <x v="13"/>
     <x v="21"/>
-    <x v="1"/>
+    <x v="7"/>
+    <x v="4"/>
+    <x v="6"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="WTIUSD_H1"/>
-    <x v="21"/>
+    <x v="6"/>
     <x v="1"/>
     <x v="0"/>
-    <n v="48486"/>
-    <x v="24"/>
-    <x v="14"/>
-    <x v="21"/>
-    <x v="1"/>
+    <x v="22"/>
+    <x v="15"/>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="WTIUSD_H4"/>
-    <x v="21"/>
+    <x v="6"/>
     <x v="2"/>
     <x v="0"/>
-    <n v="12882"/>
-    <x v="24"/>
-    <x v="15"/>
-    <x v="21"/>
-    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="WTIUSD_M1"/>
-    <x v="21"/>
+    <x v="6"/>
     <x v="3"/>
     <x v="0"/>
-    <n v="2555385"/>
-    <x v="25"/>
-    <x v="25"/>
-    <x v="21"/>
-    <x v="1"/>
+    <x v="23"/>
+    <x v="16"/>
+    <x v="14"/>
+    <x v="6"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="WTIUSD_M15"/>
-    <x v="21"/>
+    <x v="6"/>
     <x v="4"/>
     <x v="0"/>
-    <n v="190766"/>
-    <x v="25"/>
-    <x v="18"/>
-    <x v="21"/>
-    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="WTIUSD_M30"/>
-    <x v="21"/>
+    <x v="6"/>
     <x v="5"/>
     <x v="0"/>
-    <n v="95926"/>
-    <x v="24"/>
-    <x v="23"/>
-    <x v="21"/>
-    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="WTIUSD_M5"/>
-    <x v="21"/>
+    <x v="6"/>
     <x v="6"/>
     <x v="0"/>
-    <n v="565687"/>
-    <x v="25"/>
-    <x v="26"/>
-    <x v="21"/>
-    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="XAUUSD_D1"/>
-    <x v="22"/>
+    <x v="7"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="2733"/>
-    <x v="26"/>
-    <x v="0"/>
-    <x v="22"/>
-    <x v="1"/>
+    <x v="24"/>
+    <x v="17"/>
+    <x v="4"/>
+    <x v="7"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="XAUUSD_H1"/>
-    <x v="22"/>
+    <x v="7"/>
     <x v="1"/>
     <x v="0"/>
-    <n v="53215"/>
-    <x v="27"/>
-    <x v="20"/>
-    <x v="22"/>
-    <x v="1"/>
+    <x v="25"/>
+    <x v="18"/>
+    <x v="5"/>
+    <x v="7"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="XAUUSD_H4"/>
-    <x v="22"/>
+    <x v="7"/>
     <x v="2"/>
     <x v="0"/>
-    <n v="14062"/>
-    <x v="28"/>
     <x v="2"/>
-    <x v="22"/>
-    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="7"/>
+    <x v="3"/>
   </r>
   <r>
     <s v="XAUUSD_M1"/>
-    <x v="22"/>
+    <x v="7"/>
     <x v="3"/>
     <x v="0"/>
-    <n v="3441846"/>
-    <x v="27"/>
+    <x v="26"/>
+    <x v="18"/>
+    <x v="7"/>
+    <x v="7"/>
     <x v="3"/>
-    <x v="22"/>
-    <x v="1"/>
   </r>
   <r>
     <s v="XAUUSD_M15"/>
-    <x v="22"/>
+    <x v="7"/>
     <x v="4"/>
     <x v="0"/>
-    <n v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="7"/>
     <x v="3"/>
-    <x v="4"/>
-    <x v="22"/>
-    <x v="1"/>
   </r>
   <r>
     <s v="XAUUSD_M30"/>
-    <x v="22"/>
+    <x v="7"/>
     <x v="5"/>
     <x v="0"/>
-    <n v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="7"/>
     <x v="3"/>
-    <x v="4"/>
-    <x v="22"/>
-    <x v="1"/>
   </r>
   <r>
     <s v="XAUUSD_M5"/>
-    <x v="22"/>
+    <x v="7"/>
     <x v="6"/>
     <x v="0"/>
-    <n v="614568"/>
-    <x v="27"/>
-    <x v="5"/>
-    <x v="22"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="XRB_D1"/>
-    <x v="23"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="7"/>
     <x v="3"/>
-    <x v="4"/>
-    <x v="23"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="XRB_H1"/>
-    <x v="23"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="23"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="XRB_H4"/>
-    <x v="23"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="23"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="XRB_M1"/>
-    <x v="23"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="23"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="XRB_M15"/>
-    <x v="23"/>
-    <x v="4"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="23"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="XRB_M30"/>
-    <x v="23"/>
-    <x v="5"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="23"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <s v="XRB_M5"/>
-    <x v="23"/>
-    <x v="6"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="3"/>
-    <x v="4"/>
-    <x v="23"/>
-    <x v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
-  <location ref="A3:G18" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="A3:G17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
       <items count="26">
+        <item m="1" x="11"/>
+        <item m="1" x="13"/>
+        <item m="1" x="8"/>
         <item x="0"/>
         <item x="1"/>
+        <item m="1" x="23"/>
+        <item m="1" x="24"/>
         <item x="2"/>
+        <item m="1" x="16"/>
+        <item m="1" x="9"/>
+        <item m="1" x="17"/>
+        <item m="1" x="14"/>
+        <item m="1" x="15"/>
+        <item m="1" x="18"/>
+        <item m="1" x="21"/>
+        <item m="1" x="19"/>
+        <item m="1" x="12"/>
         <item x="3"/>
+        <item m="1" x="10"/>
         <item x="4"/>
         <item x="5"/>
+        <item m="1" x="22"/>
         <item x="6"/>
         <item x="7"/>
-        <item m="1" x="24"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
+        <item m="1" x="20"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5125,11 +3884,12 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item sd="0" x="3"/>
-        <item sd="0" x="1"/>
+      <items count="5">
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item m="1" x="4"/>
         <item x="0"/>
-        <item x="2"/>
       </items>
     </pivotField>
   </pivotFields>
@@ -5137,42 +3897,39 @@
     <field x="8"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="13">
+  <rowItems count="12">
     <i>
       <x/>
     </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
     <i>
       <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
     </i>
     <i>
       <x v="2"/>
     </i>
     <i r="1">
-      <x/>
-    </i>
-    <i r="1">
       <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
     </i>
     <i r="1">
       <x v="7"/>
     </i>
     <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
       <x v="20"/>
     </i>
     <i>
-      <x v="3"/>
+      <x v="4"/>
     </i>
     <i r="1">
       <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
     </i>
     <i r="1">
       <x v="17"/>
@@ -6443,7 +5200,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6455,30 +5212,30 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>480</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -6489,7 +5246,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -6500,7 +5257,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -17977,7 +16734,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="2" t="s">
@@ -17992,7 +16749,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="4" t="s">
@@ -23907,10 +22664,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23983,45 +22740,41 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>471</v>
-      </c>
-      <c r="B6" s="18">
-        <v>0</v>
-      </c>
+        <v>470</v>
+      </c>
+      <c r="B6" s="18"/>
       <c r="C6" s="35"/>
       <c r="D6" s="35"/>
-      <c r="E6" s="18">
-        <v>0</v>
-      </c>
+      <c r="E6" s="18"/>
       <c r="F6" s="35"/>
       <c r="G6" s="35"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>472</v>
+      <c r="A7" s="53" t="s">
+        <v>66</v>
       </c>
       <c r="B7" s="18">
-        <v>101701</v>
+        <v>25305</v>
       </c>
       <c r="C7" s="35">
-        <v>39887.708333333336</v>
+        <v>35898.666666666664</v>
       </c>
       <c r="D7" s="35">
-        <v>43465.625</v>
+        <v>41467.666666666664</v>
       </c>
       <c r="E7" s="18">
-        <v>5997231</v>
+        <v>544614</v>
       </c>
       <c r="F7" s="35">
-        <v>39887.708333333336</v>
+        <v>35898.627083333333</v>
       </c>
       <c r="G7" s="35">
-        <v>43465.706944444442</v>
+        <v>41467.626388888886</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="35"/>
@@ -24032,114 +22785,102 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
-        <v>2</v>
+        <v>465</v>
       </c>
       <c r="B9" s="18">
-        <v>88174</v>
+        <v>48486</v>
       </c>
       <c r="C9" s="35">
-        <v>36682.5</v>
+        <v>40496.833333333336</v>
       </c>
       <c r="D9" s="35">
-        <v>42362.5</v>
+        <v>43465.625</v>
       </c>
       <c r="E9" s="18">
-        <v>5525543</v>
+        <v>2555385</v>
       </c>
       <c r="F9" s="35">
-        <v>36682.502083333333</v>
+        <v>40496.84375</v>
       </c>
       <c r="G9" s="35">
-        <v>43465.706944444442</v>
+        <v>43465.677777777775</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="53" t="s">
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="B10" s="18">
-        <v>112933</v>
+        <v>59342</v>
       </c>
       <c r="C10" s="35">
-        <v>36676.708333333336</v>
+        <v>39887.708333333336</v>
       </c>
       <c r="D10" s="35">
         <v>43465.625</v>
       </c>
       <c r="E10" s="18">
-        <v>6160868</v>
+        <v>3447353</v>
       </c>
       <c r="F10" s="35">
-        <v>36676.727083333331</v>
+        <v>39887.708333333336</v>
       </c>
       <c r="G10" s="35">
-        <v>43465.707638888889</v>
+        <v>43465.706944444442</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
-        <v>419</v>
-      </c>
-      <c r="B11" s="18">
-        <v>60478</v>
-      </c>
-      <c r="C11" s="35">
-        <v>39537.708333333336</v>
-      </c>
-      <c r="D11" s="35">
-        <v>43098.625</v>
-      </c>
-      <c r="E11" s="18">
-        <v>3957732</v>
-      </c>
-      <c r="F11" s="35">
-        <v>39537.708333333336</v>
-      </c>
-      <c r="G11" s="35">
-        <v>43465.706944444442</v>
-      </c>
+      <c r="A11" s="16" t="s">
+        <v>469</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" s="18">
-        <v>106714</v>
+        <v>113029</v>
       </c>
       <c r="C12" s="35">
         <v>36676.708333333336</v>
       </c>
       <c r="D12" s="35">
-        <v>43098.625</v>
+        <v>43465.625</v>
       </c>
       <c r="E12" s="18">
-        <v>6046193</v>
+        <v>6166608</v>
       </c>
       <c r="F12" s="35">
-        <v>36676.749305555553</v>
+        <v>36676.727083333331</v>
       </c>
       <c r="G12" s="35">
-        <v>43465.706944444442</v>
+        <v>43465.707638888889</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="B13" s="18">
-        <v>73075</v>
+        <v>113036</v>
       </c>
       <c r="C13" s="35">
-        <v>38576.708333333336</v>
+        <v>36676.708333333336</v>
       </c>
       <c r="D13" s="35">
-        <v>43098.625</v>
+        <v>43465.625</v>
       </c>
       <c r="E13" s="18">
-        <v>4207343</v>
+        <v>6051930</v>
       </c>
       <c r="F13" s="35">
-        <v>38576.709027777775</v>
+        <v>36676.749305555553</v>
       </c>
       <c r="G13" s="35">
         <v>43465.706944444442</v>
@@ -24150,16 +22891,16 @@
         <v>68</v>
       </c>
       <c r="B14" s="18">
-        <v>106801</v>
+        <v>113123</v>
       </c>
       <c r="C14" s="35">
         <v>36676.708333333336</v>
       </c>
       <c r="D14" s="35">
-        <v>43098.625</v>
+        <v>43465.625</v>
       </c>
       <c r="E14" s="18">
-        <v>6123961</v>
+        <v>6129662</v>
       </c>
       <c r="F14" s="35">
         <v>36676.748611111114</v>
@@ -24170,7 +22911,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="35"/>
@@ -24204,39 +22945,24 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B17" s="18">
-        <v>0</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
+        <v>48996</v>
+      </c>
+      <c r="C17" s="35">
+        <v>40496.75</v>
+      </c>
+      <c r="D17" s="35">
+        <v>43465.625</v>
+      </c>
       <c r="E17" s="18">
-        <v>0</v>
-      </c>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="18">
-        <v>48996</v>
-      </c>
-      <c r="C18" s="35">
+        <v>2117667</v>
+      </c>
+      <c r="F17" s="35">
         <v>40496.75</v>
       </c>
-      <c r="D18" s="35">
-        <v>43465.625</v>
-      </c>
-      <c r="E18" s="18">
-        <v>2117667</v>
-      </c>
-      <c r="F18" s="35">
-        <v>40496.75</v>
-      </c>
-      <c r="G18" s="35">
+      <c r="G17" s="35">
         <v>43465.675694444442</v>
       </c>
     </row>
@@ -24269,7 +22995,7 @@
         <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -24277,7 +23003,7 @@
         <v>120</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>